<commit_message>
Updated data, figures, colors, etc
</commit_message>
<xml_diff>
--- a/CMA_aging_Atlas_sumdata.xlsx
+++ b/CMA_aging_Atlas_sumdata.xlsx
@@ -88,6 +88,9 @@
     <t xml:space="preserve">EC astrocytes</t>
   </si>
   <si>
+    <t xml:space="preserve">EC neurons</t>
+  </si>
+  <si>
     <t>Glomeruli</t>
   </si>
   <si>
@@ -101,9 +104,6 @@
   </si>
   <si>
     <t xml:space="preserve">Lung Fibroblasts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PC neurons</t>
   </si>
   <si>
     <t xml:space="preserve">Rods photoreceptors</t>
@@ -156,12 +156,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left style="none"/>
       <right style="none"/>
       <top style="none"/>
       <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
       <diagonal style="none"/>
     </border>
   </borders>
@@ -170,7 +185,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" quotePrefix="0" pivotButton="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="0" pivotButton="0">
+    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" quotePrefix="0" pivotButton="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -686,18 +701,16 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A85" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" min="1" max="1" width="22.61328125"/>
-    <col bestFit="1" min="2" max="2" width="12.90234375"/>
-    <col bestFit="1" min="3" max="3" width="11.6640625"/>
-    <col bestFit="1" min="4" max="4" width="10.04296875"/>
-    <col bestFit="1" min="5" max="5" width="15.6640625"/>
-    <col bestFit="1" min="6" max="6" width="10.04296875"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" width="22.61328125"/>
+    <col customWidth="1" min="2" max="4" width="12.7109375"/>
+    <col bestFit="1" customWidth="1" min="5" max="5" width="15.6640625"/>
+    <col customWidth="1" min="6" max="6" width="12.7109375"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -808,16 +821,16 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>0.093700000000000006</v>
+        <v>-1.1247</v>
       </c>
       <c r="D6">
         <v>-1.4114</v>
       </c>
       <c r="E6">
-        <v>-0.73939999999999995</v>
+        <v>-1.0761000000000001</v>
       </c>
       <c r="F6">
-        <v>1.2597</v>
+        <v>1.4666999999999999</v>
       </c>
     </row>
     <row r="7">
@@ -828,16 +841,16 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>1.077</v>
+        <v>0.34039999999999998</v>
       </c>
       <c r="D7">
         <v>0.77669999999999995</v>
       </c>
       <c r="E7">
-        <v>1.4063000000000001</v>
+        <v>0.13089999999999999</v>
       </c>
       <c r="F7">
-        <v>-1.0470999999999999</v>
+        <v>-0.48580000000000001</v>
       </c>
     </row>
     <row r="8">
@@ -848,16 +861,16 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>0.17169999999999999</v>
+        <v>1.202</v>
       </c>
       <c r="D8">
         <v>-0.0014</v>
       </c>
       <c r="E8">
-        <v>0.0224</v>
+        <v>1.3027</v>
       </c>
       <c r="F8">
-        <v>0.27729999999999999</v>
+        <v>-0.747</v>
       </c>
     </row>
     <row r="9">
@@ -868,16 +881,16 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>-1.3423</v>
+        <v>-0.41770000000000002</v>
       </c>
       <c r="D9">
         <v>0.6361</v>
       </c>
       <c r="E9">
-        <v>-0.68930000000000002</v>
+        <v>-0.35749999999999998</v>
       </c>
       <c r="F9">
-        <v>-0.4899</v>
+        <v>-0.2339</v>
       </c>
     </row>
     <row r="10">
@@ -888,16 +901,16 @@
         <v>7</v>
       </c>
       <c r="C10">
-        <v>-1.3106</v>
+        <v>-1.4755</v>
       </c>
       <c r="D10">
         <v>-1.4114</v>
       </c>
       <c r="E10">
-        <v>-1.4003000000000001</v>
+        <v>-0.29170000000000001</v>
       </c>
       <c r="F10">
-        <v>0.56279999999999997</v>
+        <v>-0.96299999999999997</v>
       </c>
     </row>
     <row r="11">
@@ -908,16 +921,16 @@
         <v>8</v>
       </c>
       <c r="C11">
-        <v>1.0778000000000001</v>
+        <v>0.32150000000000001</v>
       </c>
       <c r="D11">
         <v>0.77669999999999995</v>
       </c>
       <c r="E11">
-        <v>0.27300000000000002</v>
+        <v>0.33860000000000001</v>
       </c>
       <c r="F11">
-        <v>1.0038</v>
+        <v>-0.42420000000000002</v>
       </c>
     </row>
     <row r="12">
@@ -928,16 +941,16 @@
         <v>9</v>
       </c>
       <c r="C12">
-        <v>0.33260000000000001</v>
+        <v>0.41310000000000002</v>
       </c>
       <c r="D12">
         <v>-0.0014</v>
       </c>
       <c r="E12">
-        <v>0.96930000000000005</v>
+        <v>-1.2064999999999999</v>
       </c>
       <c r="F12">
-        <v>-0.30980000000000002</v>
+        <v>1.3756999999999999</v>
       </c>
     </row>
     <row r="13">
@@ -948,16 +961,16 @@
         <v>10</v>
       </c>
       <c r="C13">
-        <v>-0.0998</v>
+        <v>0.7409</v>
       </c>
       <c r="D13">
         <v>0.6361</v>
       </c>
       <c r="E13">
-        <v>0.158</v>
+        <v>1.1596</v>
       </c>
       <c r="F13">
-        <v>-1.2567999999999999</v>
+        <v>0.0115</v>
       </c>
     </row>
     <row r="14">
@@ -1368,16 +1381,16 @@
         <v>7</v>
       </c>
       <c r="C34">
-        <v>-0.15459999999999999</v>
+        <v>-1.1681999999999999</v>
       </c>
       <c r="D34">
         <v>-0.66639999999999999</v>
       </c>
       <c r="E34">
-        <v>-0.54900000000000004</v>
+        <v>-0.21199999999999999</v>
       </c>
       <c r="F34">
-        <v>-0.43209999999999998</v>
+        <v>-1.2033</v>
       </c>
     </row>
     <row r="35">
@@ -1388,16 +1401,16 @@
         <v>8</v>
       </c>
       <c r="C35">
-        <v>-0.96030000000000004</v>
+        <v>0.3135</v>
       </c>
       <c r="D35">
         <v>1.3182</v>
       </c>
       <c r="E35">
-        <v>0.67269999999999996</v>
+        <v>-1.2023999999999999</v>
       </c>
       <c r="F35">
-        <v>-0.13819999999999999</v>
+        <v>0.6079</v>
       </c>
     </row>
     <row r="36">
@@ -1408,16 +1421,16 @@
         <v>9</v>
       </c>
       <c r="C36">
-        <v>-0.28889999999999999</v>
+        <v>-0.33800000000000002</v>
       </c>
       <c r="D36">
         <v>-0.87629999999999997</v>
       </c>
       <c r="E36">
-        <v>-1.1196999999999999</v>
+        <v>0.20280000000000001</v>
       </c>
       <c r="F36">
-        <v>-0.8619</v>
+        <v>-0.4113</v>
       </c>
     </row>
     <row r="37">
@@ -1428,16 +1441,16 @@
         <v>10</v>
       </c>
       <c r="C37">
-        <v>1.4037999999999999</v>
+        <v>1.1928000000000001</v>
       </c>
       <c r="D37">
         <v>0.22450000000000001</v>
       </c>
       <c r="E37">
-        <v>0.99609999999999999</v>
+        <v>1.2117</v>
       </c>
       <c r="F37">
-        <v>1.4321999999999999</v>
+        <v>1.0066999999999999</v>
       </c>
     </row>
     <row r="38">
@@ -1448,13 +1461,13 @@
         <v>7</v>
       </c>
       <c r="C38">
-        <v>0.081699999999999995</v>
+        <v>-0.1623</v>
       </c>
       <c r="D38">
         <v>0.75209999999999999</v>
       </c>
       <c r="E38">
-        <v>-0.15090000000000001</v>
+        <v>-0.28999999999999998</v>
       </c>
       <c r="F38">
         <v>0.51429999999999998</v>
@@ -1468,13 +1481,13 @@
         <v>8</v>
       </c>
       <c r="C39">
-        <v>0.8891</v>
+        <v>1.0611999999999999</v>
       </c>
       <c r="D39">
         <v>-1.2020999999999999</v>
       </c>
       <c r="E39">
-        <v>1.0795999999999999</v>
+        <v>1.2299</v>
       </c>
       <c r="F39">
         <v>0.55169999999999997</v>
@@ -1488,13 +1501,13 @@
         <v>9</v>
       </c>
       <c r="C40">
-        <v>-1.4158999999999999</v>
+        <v>-1.2989999999999999</v>
       </c>
       <c r="D40">
         <v>-0.44140000000000001</v>
       </c>
       <c r="E40">
-        <v>-1.2950999999999999</v>
+        <v>-1.1634</v>
       </c>
       <c r="F40">
         <v>-1.4981</v>
@@ -1508,13 +1521,13 @@
         <v>10</v>
       </c>
       <c r="C41">
-        <v>0.4451</v>
+        <v>0.40000000000000002</v>
       </c>
       <c r="D41">
         <v>0.89139999999999997</v>
       </c>
       <c r="E41">
-        <v>0.3664</v>
+        <v>0.2235</v>
       </c>
       <c r="F41">
         <v>0.432</v>
@@ -1836,16 +1849,16 @@
         <v>7</v>
       </c>
       <c r="C58">
-        <v>-0.66349999999999998</v>
+        <v>1.2138</v>
       </c>
       <c r="D58">
-        <v>-0.68020000000000003</v>
+        <v>-1.2117</v>
       </c>
       <c r="E58">
-        <v>-0.54239999999999999</v>
+        <v>1.4528000000000001</v>
       </c>
       <c r="F58">
-        <v>-0.40350000000000003</v>
+        <v>0.64259999999999995</v>
       </c>
     </row>
     <row r="59">
@@ -1856,16 +1869,16 @@
         <v>8</v>
       </c>
       <c r="C59">
-        <v>1.3407</v>
+        <v>-0.1835</v>
       </c>
       <c r="D59">
-        <v>-0.216</v>
+        <v>0.97370000000000001</v>
       </c>
       <c r="E59">
-        <v>0.65090000000000003</v>
+        <v>-0.53010000000000002</v>
       </c>
       <c r="F59">
-        <v>1.4958</v>
+        <v>0.42349999999999999</v>
       </c>
     </row>
     <row r="60">
@@ -1876,16 +1889,16 @@
         <v>9</v>
       </c>
       <c r="C60">
-        <v>-0.85489999999999999</v>
+        <v>0.17849999999999999</v>
       </c>
       <c r="D60">
-        <v>-0.57399999999999995</v>
+        <v>-0.40810000000000002</v>
       </c>
       <c r="E60">
-        <v>-1.1211</v>
+        <v>-0.76370000000000005</v>
       </c>
       <c r="F60">
-        <v>-0.50690000000000002</v>
+        <v>0.4259</v>
       </c>
     </row>
     <row r="61">
@@ -1896,16 +1909,16 @@
         <v>10</v>
       </c>
       <c r="C61">
-        <v>0.1777</v>
+        <v>-1.2088000000000001</v>
       </c>
       <c r="D61">
-        <v>1.4701</v>
+        <v>0.64600000000000002</v>
       </c>
       <c r="E61">
-        <v>1.0125999999999999</v>
+        <v>-0.159</v>
       </c>
       <c r="F61">
-        <v>-0.58540000000000003</v>
+        <v>-1.4921</v>
       </c>
     </row>
     <row r="62">
@@ -1916,16 +1929,16 @@
         <v>7</v>
       </c>
       <c r="C62">
-        <v>-1.0027999999999999</v>
+        <v>-0.42299999999999999</v>
       </c>
       <c r="D62">
-        <v>-0.3412</v>
+        <v>-0.68020000000000003</v>
       </c>
       <c r="E62">
-        <v>-0.30649999999999999</v>
+        <v>0.14610000000000001</v>
       </c>
       <c r="F62">
-        <v>-0.73550000000000004</v>
+        <v>-0.46000000000000002</v>
       </c>
     </row>
     <row r="63">
@@ -1936,16 +1949,16 @@
         <v>8</v>
       </c>
       <c r="C63">
-        <v>0.2069</v>
+        <v>1.3512</v>
       </c>
       <c r="D63">
-        <v>0.87690000000000001</v>
+        <v>-0.216</v>
       </c>
       <c r="E63">
-        <v>1.2581</v>
+        <v>-0.0183</v>
       </c>
       <c r="F63">
-        <v>-0.67510000000000003</v>
+        <v>1.1677999999999999</v>
       </c>
     </row>
     <row r="64">
@@ -1956,16 +1969,16 @@
         <v>9</v>
       </c>
       <c r="C64">
-        <v>-0.50619999999999998</v>
+        <v>-0.99539999999999995</v>
       </c>
       <c r="D64">
-        <v>-1.2605999999999999</v>
+        <v>-0.57399999999999995</v>
       </c>
       <c r="E64">
-        <v>-1.1355</v>
+        <v>-1.2825</v>
       </c>
       <c r="F64">
-        <v>-0.0047999999999999996</v>
+        <v>-1.1202000000000001</v>
       </c>
     </row>
     <row r="65">
@@ -1976,16 +1989,16 @@
         <v>10</v>
       </c>
       <c r="C65">
-        <v>1.3021</v>
+        <v>0.067299999999999999</v>
       </c>
       <c r="D65">
-        <v>0.72489999999999999</v>
+        <v>1.4701</v>
       </c>
       <c r="E65">
-        <v>0.18390000000000001</v>
+        <v>1.1548</v>
       </c>
       <c r="F65">
-        <v>1.4154</v>
+        <v>0.4123</v>
       </c>
     </row>
     <row r="66">
@@ -1996,16 +2009,16 @@
         <v>7</v>
       </c>
       <c r="C66">
-        <v>0.40899999999999997</v>
+        <v>-1.0027999999999999</v>
       </c>
       <c r="D66">
-        <v>-0.79279999999999995</v>
+        <v>-0.3412</v>
       </c>
       <c r="E66">
-        <v>-1.0619000000000001</v>
+        <v>-0.30649999999999999</v>
       </c>
       <c r="F66">
-        <v>0.97719999999999996</v>
+        <v>-0.73550000000000004</v>
       </c>
     </row>
     <row r="67">
@@ -2016,16 +2029,16 @@
         <v>8</v>
       </c>
       <c r="C67">
-        <v>0.85750000000000004</v>
+        <v>0.2069</v>
       </c>
       <c r="D67">
-        <v>-0.36899999999999999</v>
+        <v>0.87690000000000001</v>
       </c>
       <c r="E67">
-        <v>0.58819999999999995</v>
+        <v>1.2581</v>
       </c>
       <c r="F67">
-        <v>0.2999</v>
+        <v>-0.67510000000000003</v>
       </c>
     </row>
     <row r="68">
@@ -2036,16 +2049,16 @@
         <v>9</v>
       </c>
       <c r="C68">
-        <v>0.17150000000000001</v>
+        <v>-0.50619999999999998</v>
       </c>
       <c r="D68">
-        <v>1.4641999999999999</v>
+        <v>-1.2605999999999999</v>
       </c>
       <c r="E68">
-        <v>-0.60399999999999998</v>
+        <v>-1.1355</v>
       </c>
       <c r="F68">
-        <v>0.1164</v>
+        <v>-0.0047999999999999996</v>
       </c>
     </row>
     <row r="69">
@@ -2056,16 +2069,16 @@
         <v>10</v>
       </c>
       <c r="C69">
-        <v>-1.4379999999999999</v>
+        <v>1.3021</v>
       </c>
       <c r="D69">
-        <v>-0.30249999999999999</v>
+        <v>0.72489999999999999</v>
       </c>
       <c r="E69">
-        <v>1.0777000000000001</v>
+        <v>0.18390000000000001</v>
       </c>
       <c r="F69">
-        <v>-1.3934</v>
+        <v>1.4154</v>
       </c>
     </row>
     <row r="70">
@@ -2076,16 +2089,16 @@
         <v>7</v>
       </c>
       <c r="C70">
-        <v>-0.063700000000000007</v>
+        <v>0.40899999999999997</v>
       </c>
       <c r="D70">
-        <v>0.54449999999999998</v>
+        <v>-0.79279999999999995</v>
       </c>
       <c r="E70">
-        <v>-0.8589</v>
+        <v>-1.0619000000000001</v>
       </c>
       <c r="F70">
-        <v>1.2359</v>
+        <v>0.97719999999999996</v>
       </c>
     </row>
     <row r="71">
@@ -2096,16 +2109,16 @@
         <v>8</v>
       </c>
       <c r="C71">
-        <v>-1.0249999999999999</v>
+        <v>0.85750000000000004</v>
       </c>
       <c r="D71">
-        <v>-0.84889999999999999</v>
+        <v>-0.36899999999999999</v>
       </c>
       <c r="E71">
-        <v>0.018200000000000001</v>
+        <v>0.58819999999999995</v>
       </c>
       <c r="F71">
-        <v>-0.67959999999999998</v>
+        <v>0.2999</v>
       </c>
     </row>
     <row r="72">
@@ -2116,16 +2129,16 @@
         <v>9</v>
       </c>
       <c r="C72">
-        <v>-0.27800000000000002</v>
+        <v>0.17150000000000001</v>
       </c>
       <c r="D72">
-        <v>-0.83179999999999998</v>
+        <v>1.4641999999999999</v>
       </c>
       <c r="E72">
-        <v>-0.55649999999999999</v>
+        <v>-0.60399999999999998</v>
       </c>
       <c r="F72">
-        <v>0.37609999999999999</v>
+        <v>0.1164</v>
       </c>
     </row>
     <row r="73">
@@ -2136,16 +2149,16 @@
         <v>10</v>
       </c>
       <c r="C73">
-        <v>1.3667</v>
+        <v>-1.4379999999999999</v>
       </c>
       <c r="D73">
-        <v>1.1362000000000001</v>
+        <v>-0.30249999999999999</v>
       </c>
       <c r="E73">
-        <v>1.3972</v>
+        <v>1.0777000000000001</v>
       </c>
       <c r="F73">
-        <v>-0.93240000000000001</v>
+        <v>-1.3934</v>
       </c>
     </row>
     <row r="74">
@@ -2156,16 +2169,16 @@
         <v>7</v>
       </c>
       <c r="C74">
-        <v>-0.92810000000000004</v>
+        <v>0.1108</v>
       </c>
       <c r="D74">
-        <v>1.0763</v>
+        <v>0.54449999999999998</v>
       </c>
       <c r="E74">
-        <v>-1.1896</v>
+        <v>-1.0895999999999999</v>
       </c>
       <c r="F74">
-        <v>-0.94310000000000005</v>
+        <v>1.3954</v>
       </c>
     </row>
     <row r="75">
@@ -2176,16 +2189,16 @@
         <v>8</v>
       </c>
       <c r="C75">
-        <v>1.3976</v>
+        <v>-0.92710000000000004</v>
       </c>
       <c r="D75">
-        <v>-0.82169999999999999</v>
+        <v>-0.84889999999999999</v>
       </c>
       <c r="E75">
-        <v>1.0245</v>
+        <v>-0.16689999999999999</v>
       </c>
       <c r="F75">
-        <v>1.4137999999999999</v>
+        <v>-0.81430000000000002</v>
       </c>
     </row>
     <row r="76">
@@ -2196,16 +2209,16 @@
         <v>9</v>
       </c>
       <c r="C76">
-        <v>-0.42849999999999999</v>
+        <v>-0.53920000000000001</v>
       </c>
       <c r="D76">
-        <v>-0.88029999999999997</v>
+        <v>-0.83179999999999998</v>
       </c>
       <c r="E76">
-        <v>-0.42820000000000003</v>
+        <v>-0.077100000000000002</v>
       </c>
       <c r="F76">
-        <v>-0.21310000000000001</v>
+        <v>-0.62280000000000002</v>
       </c>
     </row>
     <row r="77">
@@ -2216,16 +2229,16 @@
         <v>10</v>
       </c>
       <c r="C77">
-        <v>-0.040899999999999999</v>
+        <v>1.3554999999999999</v>
       </c>
       <c r="D77">
-        <v>0.62570000000000003</v>
+        <v>1.1362000000000001</v>
       </c>
       <c r="E77">
-        <v>0.59319999999999995</v>
+        <v>1.3337000000000001</v>
       </c>
       <c r="F77">
-        <v>-0.25769999999999998</v>
+        <v>0.041700000000000001</v>
       </c>
     </row>
     <row r="78">
@@ -2236,16 +2249,16 @@
         <v>7</v>
       </c>
       <c r="C78">
-        <v>0.77190000000000003</v>
+        <v>-1.0174000000000001</v>
       </c>
       <c r="D78">
-        <v>-1.2117</v>
+        <v>1.0763</v>
       </c>
       <c r="E78">
-        <v>0.6018</v>
+        <v>-1.0976999999999999</v>
       </c>
       <c r="F78">
-        <v>0.55110000000000003</v>
+        <v>-0.83640000000000003</v>
       </c>
     </row>
     <row r="79">
@@ -2256,16 +2269,16 @@
         <v>8</v>
       </c>
       <c r="C79">
-        <v>0.9496</v>
+        <v>1.1988000000000001</v>
       </c>
       <c r="D79">
-        <v>0.97370000000000001</v>
+        <v>-0.82169999999999999</v>
       </c>
       <c r="E79">
-        <v>0.96279999999999999</v>
+        <v>0.70130000000000003</v>
       </c>
       <c r="F79">
-        <v>1.1059000000000001</v>
+        <v>1.4482999999999999</v>
       </c>
     </row>
     <row r="80">
@@ -2276,16 +2289,16 @@
         <v>9</v>
       </c>
       <c r="C80">
-        <v>-0.96230000000000004</v>
+        <v>-0.59630000000000005</v>
       </c>
       <c r="D80">
-        <v>-0.40810000000000002</v>
+        <v>-0.88029999999999997</v>
       </c>
       <c r="E80">
-        <v>-1.2757000000000001</v>
+        <v>-0.58440000000000003</v>
       </c>
       <c r="F80">
-        <v>-1.0527</v>
+        <v>-0.3947</v>
       </c>
     </row>
     <row r="81">
@@ -2296,16 +2309,16 @@
         <v>10</v>
       </c>
       <c r="C81">
-        <v>-0.75919999999999999</v>
+        <v>0.41499999999999998</v>
       </c>
       <c r="D81">
-        <v>0.64600000000000002</v>
+        <v>0.62570000000000003</v>
       </c>
       <c r="E81">
-        <v>-0.2888</v>
+        <v>0.98070000000000002</v>
       </c>
       <c r="F81">
-        <v>-0.60429999999999995</v>
+        <v>-0.2172</v>
       </c>
     </row>
     <row r="82">
@@ -2544,16 +2557,16 @@
         <v>7</v>
       </c>
       <c r="C94">
-        <v>-0.71360000000000001</v>
+        <v>-0.69140000000000001</v>
       </c>
       <c r="D94">
         <v>0.92869999999999997</v>
       </c>
       <c r="E94">
-        <v>-0.73280000000000001</v>
+        <v>-0.79149999999999998</v>
       </c>
       <c r="F94">
-        <v>1.1609</v>
+        <v>0.69840000000000002</v>
       </c>
     </row>
     <row r="95">
@@ -2564,16 +2577,16 @@
         <v>8</v>
       </c>
       <c r="C95">
-        <v>1.1151</v>
+        <v>1.3439000000000001</v>
       </c>
       <c r="D95">
         <v>-0.0361</v>
       </c>
       <c r="E95">
-        <v>1.1293</v>
+        <v>0.99070000000000003</v>
       </c>
       <c r="F95">
-        <v>-0.65200000000000002</v>
+        <v>-0.080500000000000002</v>
       </c>
     </row>
     <row r="96">
@@ -2584,16 +2597,16 @@
         <v>9</v>
       </c>
       <c r="C96">
-        <v>-0.96450000000000002</v>
+        <v>-0.82779999999999998</v>
       </c>
       <c r="D96">
         <v>-1.3785000000000001</v>
       </c>
       <c r="E96">
-        <v>-0.94289999999999996</v>
+        <v>-0.92789999999999995</v>
       </c>
       <c r="F96">
-        <v>0.48649999999999999</v>
+        <v>0.76690000000000003</v>
       </c>
     </row>
     <row r="97">
@@ -2604,16 +2617,16 @@
         <v>10</v>
       </c>
       <c r="C97">
-        <v>0.56299999999999994</v>
+        <v>0.17519999999999999</v>
       </c>
       <c r="D97">
         <v>0.48580000000000001</v>
       </c>
       <c r="E97">
-        <v>0.5464</v>
+        <v>0.72870000000000001</v>
       </c>
       <c r="F97">
-        <v>-0.99529999999999996</v>
+        <v>-1.3848</v>
       </c>
     </row>
     <row r="98">
@@ -2624,16 +2637,16 @@
         <v>7</v>
       </c>
       <c r="C98">
-        <v>0.46889999999999998</v>
+        <v>0.37509999999999999</v>
       </c>
       <c r="D98">
         <v>0.54759999999999998</v>
       </c>
       <c r="E98">
-        <v>0.56789999999999996</v>
+        <v>0.37140000000000001</v>
       </c>
       <c r="F98">
-        <v>-0.3574</v>
+        <v>-0.35780000000000001</v>
       </c>
     </row>
     <row r="99">
@@ -2644,16 +2657,16 @@
         <v>8</v>
       </c>
       <c r="C99">
-        <v>0.89410000000000001</v>
+        <v>0.85150000000000003</v>
       </c>
       <c r="D99">
         <v>-1.4890000000000001</v>
       </c>
       <c r="E99">
-        <v>0.59689999999999999</v>
+        <v>0.63870000000000005</v>
       </c>
       <c r="F99">
-        <v>1.2381</v>
+        <v>1.2383</v>
       </c>
     </row>
     <row r="100">
@@ -2664,16 +2677,16 @@
         <v>9</v>
       </c>
       <c r="C100">
-        <v>-1.4067000000000001</v>
+        <v>-1.4446000000000001</v>
       </c>
       <c r="D100">
         <v>0.32940000000000003</v>
       </c>
       <c r="E100">
-        <v>-1.4886999999999999</v>
+        <v>-1.4908999999999999</v>
       </c>
       <c r="F100">
-        <v>-1.1301000000000001</v>
+        <v>-1.1297999999999999</v>
       </c>
     </row>
     <row r="101">
@@ -2684,16 +2697,16 @@
         <v>10</v>
       </c>
       <c r="C101">
-        <v>0.043700000000000003</v>
+        <v>0.21790000000000001</v>
       </c>
       <c r="D101">
         <v>0.61199999999999999</v>
       </c>
       <c r="E101">
-        <v>0.32390000000000002</v>
+        <v>0.48080000000000001</v>
       </c>
       <c r="F101">
-        <v>0.24940000000000001</v>
+        <v>0.2492</v>
       </c>
     </row>
     <row r="102">

</xml_diff>